<commit_message>
new approach to including variables that easily allows summing them across lines and subscripts, switch to new lookup table format, use this new approach to easily pull critical care beds instead of hardcoding them in the code, calculate medicare operating cost-to-charge ratio, fix occasional bug in flagging synthetic years with under- or over-coverage
</commit_message>
<xml_diff>
--- a/lookup.xlsx
+++ b/lookup.xlsx
@@ -1,32 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDB235-06AF-0446-8F32-CB168800FCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE23CF0-B46D-5B46-99B2-E3014DCC8FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11600" yWindow="2380" windowWidth="18640" windowHeight="16120" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15180" windowHeight="17720" activeTab="1" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
     <sheet name="Type and Label" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="168">
   <si>
     <t>rec</t>
   </si>
@@ -37,9 +47,6 @@
     <t>clmn_num</t>
   </si>
   <si>
-    <t>line_num</t>
-  </si>
-  <si>
     <t>fmt</t>
   </si>
   <si>
@@ -413,6 +420,126 @@
   </si>
   <si>
     <t>cost of patients approved for charity care and uninsured discounts (2010 format only)</t>
+  </si>
+  <si>
+    <t>05300</t>
+  </si>
+  <si>
+    <t>20200</t>
+  </si>
+  <si>
+    <t>D10A181</t>
+  </si>
+  <si>
+    <t>04200</t>
+  </si>
+  <si>
+    <t>prog_nursery_cost</t>
+  </si>
+  <si>
+    <t>prog_op_cost</t>
+  </si>
+  <si>
+    <t>D30A180</t>
+  </si>
+  <si>
+    <t>prog_net_chg</t>
+  </si>
+  <si>
+    <t>0500</t>
+  </si>
+  <si>
+    <t>D40A180</t>
+  </si>
+  <si>
+    <t>10300</t>
+  </si>
+  <si>
+    <t>line_num_end</t>
+  </si>
+  <si>
+    <t>line_num_start</t>
+  </si>
+  <si>
+    <t>02619</t>
+  </si>
+  <si>
+    <t>02719</t>
+  </si>
+  <si>
+    <t>02819</t>
+  </si>
+  <si>
+    <t>02919</t>
+  </si>
+  <si>
+    <t>02159</t>
+  </si>
+  <si>
+    <t>02080</t>
+  </si>
+  <si>
+    <t>02099</t>
+  </si>
+  <si>
+    <t>02060</t>
+  </si>
+  <si>
+    <t>02079</t>
+  </si>
+  <si>
+    <t>02180</t>
+  </si>
+  <si>
+    <t>02199</t>
+  </si>
+  <si>
+    <t>02040</t>
+  </si>
+  <si>
+    <t>02059</t>
+  </si>
+  <si>
+    <t>02120</t>
+  </si>
+  <si>
+    <t>02139</t>
+  </si>
+  <si>
+    <t>00899</t>
+  </si>
+  <si>
+    <t>00999</t>
+  </si>
+  <si>
+    <t>01099</t>
+  </si>
+  <si>
+    <t>01199</t>
+  </si>
+  <si>
+    <t>01299</t>
+  </si>
+  <si>
+    <t>03099</t>
+  </si>
+  <si>
+    <t>03599</t>
+  </si>
+  <si>
+    <t>prog_rt_chg</t>
+  </si>
+  <si>
+    <t>medicare inpatient program nursery cost</t>
+  </si>
+  <si>
+    <t>medicare inpatient program operating cost</t>
+  </si>
+  <si>
+    <t>medicare inpatient program routine service charges</t>
+  </si>
+  <si>
+    <t>medicare inpatient program ancillary service net charges</t>
   </si>
 </sst>
 </file>
@@ -765,21 +892,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,1455 +917,1708 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20">
-        <v>10</v>
-      </c>
       <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
       <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
       <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29">
-        <v>10</v>
+        <v>49</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30">
-        <v>10</v>
+        <v>56</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32">
-        <v>10</v>
+        <v>115</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34">
-        <v>10</v>
-      </c>
       <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>9</v>
+        <v>133</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42">
-        <v>96</v>
+        <v>44</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E48">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E49">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E50">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E51">
-        <v>96</v>
-      </c>
       <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="F52">
-        <v>1</v>
-      </c>
-      <c r="G52" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E53">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E54">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="F54">
-        <v>1</v>
-      </c>
-      <c r="G54" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="G56" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E57">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="F57">
+        <v>96</v>
+      </c>
+      <c r="G57">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E58">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="F59">
+        <v>96</v>
+      </c>
+      <c r="G59">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E63">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="F63">
+        <v>96</v>
+      </c>
+      <c r="G63">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E64">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="F64">
+        <v>96</v>
+      </c>
+      <c r="G64">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E65">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="G65" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E66">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E67">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="F67">
-        <v>1</v>
-      </c>
-      <c r="G67" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E68">
-        <v>96</v>
+        <v>73</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="F68">
-        <v>1</v>
-      </c>
-      <c r="G68" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E69">
-        <v>96</v>
+        <v>74</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="F69">
+        <v>96</v>
+      </c>
+      <c r="G69">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F70">
+        <v>96</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F71">
+        <v>96</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F72">
+        <v>96</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F73">
+        <v>96</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F74">
+        <v>96</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75">
+        <v>96</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F76">
+        <v>96</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F77">
+        <v>96</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F78">
+        <v>96</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E70">
-        <v>96</v>
-      </c>
-      <c r="F70">
+      <c r="F79">
+        <v>96</v>
+      </c>
+      <c r="G79">
         <v>0</v>
       </c>
-      <c r="G70" s="1"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F80">
+        <v>96</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F81">
+        <v>96</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F82">
+        <v>96</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F83">
+        <v>96</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2248,10 +2628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2266,439 +2646,483 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow processing of alpha file
</commit_message>
<xml_diff>
--- a/lookup.xlsx
+++ b/lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE23CF0-B46D-5B46-99B2-E3014DCC8FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABC5690-9172-4C47-AE6E-665EB23FB0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15180" windowHeight="17720" activeTab="1" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15180" windowHeight="17720" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="175">
   <si>
     <t>rec</t>
   </si>
@@ -540,6 +540,27 @@
   </si>
   <si>
     <t>medicare inpatient program ancillary service net charges</t>
+  </si>
+  <si>
+    <t>S200001</t>
+  </si>
+  <si>
+    <t>14100</t>
+  </si>
+  <si>
+    <t>chain_name</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>name of chain organization</t>
+  </si>
+  <si>
+    <t>S200000</t>
+  </si>
+  <si>
+    <t>04001</t>
   </si>
 </sst>
 </file>
@@ -596,9 +617,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -636,7 +657,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -742,7 +763,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -884,7 +905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -892,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:G110"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,19 +1810,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>5</v>
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
+        <v>168</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>169</v>
       </c>
       <c r="F44">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -1809,7 +1830,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>5</v>
@@ -1818,7 +1839,7 @@
         <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F45">
         <v>96</v>
@@ -1829,7 +1850,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>5</v>
@@ -1838,7 +1859,7 @@
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F46">
         <v>96</v>
@@ -1849,7 +1870,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
@@ -1858,7 +1879,7 @@
         <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F47">
         <v>96</v>
@@ -1869,7 +1890,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
@@ -1878,7 +1899,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F48">
         <v>96</v>
@@ -1889,7 +1910,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -1898,7 +1919,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F49">
         <v>96</v>
@@ -1909,16 +1930,16 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F50">
         <v>96</v>
@@ -1929,7 +1950,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>19</v>
@@ -1938,7 +1959,7 @@
         <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="F51">
         <v>96</v>
@@ -1949,7 +1970,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>19</v>
@@ -1958,7 +1979,7 @@
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F52">
         <v>96</v>
@@ -1969,7 +1990,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>19</v>
@@ -1978,7 +1999,7 @@
         <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F53">
         <v>96</v>
@@ -1989,7 +2010,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>19</v>
@@ -1998,7 +2019,7 @@
         <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F54">
         <v>96</v>
@@ -2009,7 +2030,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>19</v>
@@ -2018,7 +2039,7 @@
         <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F55">
         <v>96</v>
@@ -2029,7 +2050,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>19</v>
@@ -2038,7 +2059,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F56">
         <v>96</v>
@@ -2049,16 +2070,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F57">
         <v>96</v>
@@ -2069,7 +2090,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>19</v>
@@ -2078,7 +2099,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F58">
         <v>96</v>
@@ -2089,7 +2110,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>19</v>
@@ -2098,7 +2119,7 @@
         <v>57</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F59">
         <v>96</v>
@@ -2109,13 +2130,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>9</v>
@@ -2129,16 +2150,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="F61">
         <v>96</v>
@@ -2149,7 +2170,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>37</v>
@@ -2158,7 +2179,7 @@
         <v>55</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="F62">
         <v>96</v>
@@ -2169,16 +2190,16 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="F63">
         <v>96</v>
@@ -2189,13 +2210,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>6</v>
@@ -2209,13 +2230,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>6</v>
@@ -2229,13 +2250,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>6</v>
@@ -2249,16 +2270,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="F67">
         <v>96</v>
@@ -2269,7 +2290,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>46</v>
@@ -2278,10 +2299,7 @@
         <v>55</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="F68">
         <v>96</v>
@@ -2292,7 +2310,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>46</v>
@@ -2301,10 +2319,10 @@
         <v>55</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F69">
         <v>96</v>
@@ -2315,7 +2333,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>46</v>
@@ -2324,10 +2342,10 @@
         <v>55</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F70">
         <v>96</v>
@@ -2338,7 +2356,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>46</v>
@@ -2347,10 +2365,10 @@
         <v>55</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F71">
         <v>96</v>
@@ -2361,7 +2379,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>46</v>
@@ -2370,10 +2388,10 @@
         <v>55</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F72">
         <v>96</v>
@@ -2393,10 +2411,10 @@
         <v>55</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F73">
         <v>96</v>
@@ -2416,10 +2434,10 @@
         <v>55</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F74">
         <v>96</v>
@@ -2439,10 +2457,10 @@
         <v>55</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F75">
         <v>96</v>
@@ -2462,10 +2480,10 @@
         <v>55</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F76">
         <v>96</v>
@@ -2485,10 +2503,10 @@
         <v>55</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F77">
         <v>96</v>
@@ -2499,7 +2517,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>46</v>
@@ -2508,7 +2526,10 @@
         <v>55</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>64</v>
+        <v>154</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="F78">
         <v>96</v>
@@ -2519,36 +2540,36 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F79">
         <v>96</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>130</v>
+        <v>37</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="F80">
         <v>96</v>
@@ -2559,39 +2580,36 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F81">
         <v>96</v>
       </c>
       <c r="G81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="F82">
         <v>96</v>
@@ -2602,7 +2620,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>137</v>
@@ -2611,12 +2629,55 @@
         <v>57</v>
       </c>
       <c r="D83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F83">
+        <v>96</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F83">
-        <v>96</v>
-      </c>
-      <c r="G83">
+      <c r="F84">
+        <v>96</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F85">
+        <v>96</v>
+      </c>
+      <c r="G85">
         <v>1</v>
       </c>
     </row>
@@ -2628,10 +2689,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3125,6 +3186,17 @@
         <v>167</v>
       </c>
     </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
include hospital name and typ control in lookup
</commit_message>
<xml_diff>
--- a/lookup.xlsx
+++ b/lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asacarny/Repositories/hospital-cost-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABC5690-9172-4C47-AE6E-665EB23FB0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA14F41D-D4A4-0641-AA77-13E05DC77C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15180" windowHeight="17720" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
+    <workbookView xWindow="160" yWindow="500" windowWidth="13080" windowHeight="19860" xr2:uid="{2FC29EAB-8935-714F-80E4-2DC39A71C1EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="181">
   <si>
     <t>rec</t>
   </si>
@@ -561,6 +561,24 @@
   </si>
   <si>
     <t>04001</t>
+  </si>
+  <si>
+    <t>typ_control</t>
+  </si>
+  <si>
+    <t>hospital_name</t>
+  </si>
+  <si>
+    <t>type of control</t>
+  </si>
+  <si>
+    <t>name of hospital</t>
+  </si>
+  <si>
+    <t>beds_grandtotal</t>
+  </si>
+  <si>
+    <t>beds - grand total (total + subprovider/snf/nf/hospice)</t>
   </si>
 </sst>
 </file>
@@ -913,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2BB4DF-E65D-224C-B8BB-1875153B4956}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1627,27 +1645,27 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F35">
         <v>10</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>37</v>
@@ -1656,38 +1674,38 @@
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F36">
         <v>10</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F37">
         <v>10</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>37</v>
@@ -1696,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F38">
         <v>10</v>
@@ -1707,7 +1725,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>37</v>
@@ -1716,7 +1734,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F39">
         <v>10</v>
@@ -1727,16 +1745,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>37</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>131</v>
+        <v>75</v>
       </c>
       <c r="F40">
         <v>10</v>
@@ -1747,39 +1765,36 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F41">
         <v>10</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="F42">
         <v>10</v>
@@ -1790,7 +1805,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>134</v>
@@ -1799,7 +1814,10 @@
         <v>32</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>129</v>
+        <v>44</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="F43">
         <v>10</v>
@@ -1810,16 +1828,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B44" t="s">
-        <v>168</v>
+        <v>135</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="F44">
         <v>10</v>
@@ -1830,19 +1848,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>5</v>
+        <v>175</v>
+      </c>
+      <c r="B45" t="s">
+        <v>168</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="F45">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -1850,19 +1868,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>5</v>
+        <v>176</v>
+      </c>
+      <c r="B46" t="s">
+        <v>168</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F46">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -1870,19 +1888,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>5</v>
+        <v>170</v>
+      </c>
+      <c r="B47" t="s">
+        <v>168</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="F47">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -1890,7 +1908,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
@@ -1899,7 +1917,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="F48">
         <v>96</v>
@@ -1910,7 +1928,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -1919,7 +1937,7 @@
         <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F49">
         <v>96</v>
@@ -1930,7 +1948,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>5</v>
@@ -1939,7 +1957,7 @@
         <v>55</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F50">
         <v>96</v>
@@ -1950,16 +1968,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="F51">
         <v>96</v>
@@ -1970,16 +1988,16 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="F52">
         <v>96</v>
@@ -1990,16 +2008,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F53">
         <v>96</v>
@@ -2010,7 +2028,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>19</v>
@@ -2019,7 +2037,7 @@
         <v>55</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F54">
         <v>96</v>
@@ -2030,7 +2048,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>19</v>
@@ -2039,7 +2057,7 @@
         <v>55</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="F55">
         <v>96</v>
@@ -2050,7 +2068,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>19</v>
@@ -2059,7 +2077,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="F56">
         <v>96</v>
@@ -2070,7 +2088,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>19</v>
@@ -2079,7 +2097,7 @@
         <v>55</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F57">
         <v>96</v>
@@ -2090,13 +2108,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>25</v>
@@ -2110,13 +2128,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>27</v>
@@ -2130,13 +2148,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>9</v>
@@ -2150,16 +2168,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F61">
         <v>96</v>
@@ -2170,16 +2188,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="F62">
         <v>96</v>
@@ -2190,16 +2208,16 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="F63">
         <v>96</v>
@@ -2210,16 +2228,16 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F64">
         <v>96</v>
@@ -2230,16 +2248,16 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="F65">
         <v>96</v>
@@ -2250,16 +2268,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="F66">
         <v>96</v>
@@ -2270,13 +2288,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>6</v>
@@ -2290,16 +2308,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="F68">
         <v>96</v>
@@ -2310,19 +2328,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>141</v>
+        <v>6</v>
       </c>
       <c r="F69">
         <v>96</v>
@@ -2333,19 +2348,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="F70">
         <v>96</v>
@@ -2356,7 +2368,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>46</v>
@@ -2365,10 +2377,7 @@
         <v>55</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>143</v>
+        <v>63</v>
       </c>
       <c r="F71">
         <v>96</v>
@@ -2379,7 +2388,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>46</v>
@@ -2388,10 +2397,10 @@
         <v>55</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F72">
         <v>96</v>
@@ -2402,7 +2411,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>46</v>
@@ -2411,10 +2420,10 @@
         <v>55</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F73">
         <v>96</v>
@@ -2425,7 +2434,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>46</v>
@@ -2434,10 +2443,10 @@
         <v>55</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F74">
         <v>96</v>
@@ -2448,7 +2457,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>46</v>
@@ -2457,10 +2466,10 @@
         <v>55</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F75">
         <v>96</v>
@@ -2480,10 +2489,10 @@
         <v>55</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F76">
         <v>96</v>
@@ -2503,10 +2512,10 @@
         <v>55</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F77">
         <v>96</v>
@@ -2526,10 +2535,10 @@
         <v>55</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F78">
         <v>96</v>
@@ -2540,7 +2549,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>46</v>
@@ -2549,7 +2558,10 @@
         <v>55</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>64</v>
+        <v>150</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F79">
         <v>96</v>
@@ -2560,56 +2572,62 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>77</v>
+        <v>152</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="F80">
         <v>96</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>131</v>
+        <v>154</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="F81">
         <v>96</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="F82">
         <v>96</v>
@@ -2620,20 +2638,17 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="F83">
         <v>96</v>
       </c>
@@ -2643,41 +2658,164 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>135</v>
+        <v>76</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>137</v>
+        <v>37</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
       <c r="F84">
         <v>96</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F85">
+        <v>96</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F86">
+        <v>96</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F87">
+        <v>96</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F88">
+        <v>96</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" t="s">
+        <v>173</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F89">
+        <v>96</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F90">
+        <v>96</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B91" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F85">
-        <v>96</v>
-      </c>
-      <c r="G85">
+      <c r="F91">
+        <v>96</v>
+      </c>
+      <c r="G91">
         <v>1</v>
       </c>
     </row>
@@ -2689,10 +2827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01AFD1-3AE8-2C43-8863-F91A96C0A348}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3078,123 +3216,156 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>127</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>